<commit_message>
add comment to location and location-supported-capactity f4b537031330a8ca7a29f04720875692b8dec18f
</commit_message>
<xml_diff>
--- a/sg/ajouter-le-champ-commentaire/ig/StructureDefinition-ror-organization-price.xlsx
+++ b/sg/ajouter-le-champ-commentaire/ig/StructureDefinition-ror-organization-price.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3072" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2905" uniqueCount="238">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-14T14:30:30+00:00</t>
+    <t>2025-10-14T14:38:25+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -736,27 +736,6 @@
   </si>
   <si>
     <t>TarifPrestationSupplementaire.nomPrestationSupp</t>
-  </si>
-  <si>
-    <t>Extension.extension:comment</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>Extension.extension:comment.id</t>
-  </si>
-  <si>
-    <t>Extension.extension:comment.extension</t>
-  </si>
-  <si>
-    <t>Extension.extension:comment.url</t>
-  </si>
-  <si>
-    <t>Extension.extension:comment.value[x]</t>
-  </si>
-  <si>
-    <t>Commentaire</t>
   </si>
   <si>
     <t>base64Binary
@@ -1071,7 +1050,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL91"/>
+  <dimension ref="A1:AL86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -10081,20 +10060,18 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>237</v>
+        <v>110</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="C85" t="s" s="2">
-        <v>238</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C85" s="2"/>
       <c r="D85" t="s" s="2">
         <v>76</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85" t="s" s="2">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="G85" t="s" s="2">
         <v>84</v>
@@ -10109,22 +10086,24 @@
         <v>76</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="M85" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="N85" s="2"/>
+        <v>108</v>
+      </c>
+      <c r="N85" t="s" s="2">
+        <v>109</v>
+      </c>
       <c r="O85" s="2"/>
       <c r="P85" t="s" s="2">
         <v>76</v>
       </c>
       <c r="Q85" s="2"/>
       <c r="R85" t="s" s="2">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="S85" t="s" s="2">
         <v>76</v>
@@ -10166,33 +10145,33 @@
         <v>76</v>
       </c>
       <c r="AF85" t="s" s="2">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="AG85" t="s" s="2">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="AH85" t="s" s="2">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="AI85" t="s" s="2">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="AJ85" t="s" s="2">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="AK85" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL85" t="s" s="2">
-        <v>76</v>
+        <v>111</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s" s="2">
-        <v>239</v>
+        <v>119</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" t="s" s="2">
@@ -10203,7 +10182,7 @@
         <v>77</v>
       </c>
       <c r="G86" t="s" s="2">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="H86" t="s" s="2">
         <v>76</v>
@@ -10215,13 +10194,13 @@
         <v>76</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>85</v>
+        <v>237</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="M86" t="s" s="2">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="N86" s="2"/>
       <c r="O86" s="2"/>
@@ -10272,7 +10251,7 @@
         <v>76</v>
       </c>
       <c r="AF86" t="s" s="2">
-        <v>88</v>
+        <v>119</v>
       </c>
       <c r="AG86" t="s" s="2">
         <v>77</v>
@@ -10281,549 +10260,15 @@
         <v>84</v>
       </c>
       <c r="AI86" t="s" s="2">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AJ86" t="s" s="2">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="AK86" t="s" s="2">
         <v>76</v>
       </c>
       <c r="AL86" t="s" s="2">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="B87" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="C87" s="2"/>
-      <c r="D87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="E87" s="2"/>
-      <c r="F87" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="G87" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="H87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K87" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="L87" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="M87" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="N87" s="2"/>
-      <c r="O87" s="2"/>
-      <c r="P87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Q87" s="2"/>
-      <c r="R87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB87" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="AC87" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="AD87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE87" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="AF87" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="AG87" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH87" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI87" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AJ87" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AK87" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL87" t="s" s="2">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="B88" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="C88" s="2"/>
-      <c r="D88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="E88" s="2"/>
-      <c r="F88" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="G88" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="H88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K88" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="L88" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="M88" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="N88" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="O88" s="2"/>
-      <c r="P88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Q88" s="2"/>
-      <c r="R88" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="S88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF88" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="AG88" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AH88" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AI88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AJ88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AK88" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL88" t="s" s="2">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="B89" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="C89" s="2"/>
-      <c r="D89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="E89" s="2"/>
-      <c r="F89" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="G89" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="H89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K89" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="L89" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="M89" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="N89" s="2"/>
-      <c r="O89" s="2"/>
-      <c r="P89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Q89" s="2"/>
-      <c r="R89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE89" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF89" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="AG89" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH89" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AI89" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AJ89" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="AK89" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="AL89" t="s" s="2">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="B90" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="C90" s="2"/>
-      <c r="D90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="E90" s="2"/>
-      <c r="F90" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="G90" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="H90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K90" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="L90" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="M90" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="N90" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="O90" s="2"/>
-      <c r="P90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Q90" s="2"/>
-      <c r="R90" t="s" s="2">
-        <v>3</v>
-      </c>
-      <c r="S90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF90" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="AG90" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AH90" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AI90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AJ90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AK90" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL90" t="s" s="2">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="B91" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="C91" s="2"/>
-      <c r="D91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="E91" s="2"/>
-      <c r="F91" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="G91" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="H91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="I91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="J91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K91" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="L91" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="M91" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="N91" s="2"/>
-      <c r="O91" s="2"/>
-      <c r="P91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Q91" s="2"/>
-      <c r="R91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="S91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="T91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="U91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="V91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="W91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="X91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Z91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AA91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF91" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="AG91" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AH91" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AI91" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AJ91" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="AK91" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL91" t="s" s="2">
         <v>111</v>
       </c>
     </row>

</xml_diff>